<commit_message>
modifications to dashboard file and corrects coord of ponto 63
</commit_message>
<xml_diff>
--- a/features_pontos.xlsx
+++ b/features_pontos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos Mac\ASistemas\Projetos DS\balne_floripa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos Mac\ASistemas\Projetos DS\balne_floripa_andhros\Balneabilidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA1BC5B-B684-44E9-A38B-DEEC88C91296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730083AD-87E0-42FA-B397-1DBDEA371D50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1140" windowWidth="21600" windowHeight="11256" xr2:uid="{29C16FCB-0CAF-4187-9E1B-11F8BF6F8A37}"/>
+    <workbookView xWindow="828" yWindow="1140" windowWidth="21600" windowHeight="11112" xr2:uid="{29C16FCB-0CAF-4187-9E1B-11F8BF6F8A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1609,10 +1609,10 @@
         <v>57</v>
       </c>
       <c r="D28">
-        <v>-27.759889000000001</v>
+        <v>-27.759910000000001</v>
       </c>
       <c r="E28">
-        <v>-48.522767999999999</v>
+        <v>-48.572752000000001</v>
       </c>
       <c r="F28" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
corrects long of ponto 1
</commit_message>
<xml_diff>
--- a/features_pontos.xlsx
+++ b/features_pontos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos Mac\ASistemas\Projetos DS\balne_floripa_andhros\Balneabilidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730083AD-87E0-42FA-B397-1DBDEA371D50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38B8B31-B7CA-4E66-B59F-692DDACB46D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="1140" windowWidth="21600" windowHeight="11112" xr2:uid="{29C16FCB-0CAF-4187-9E1B-11F8BF6F8A37}"/>
+    <workbookView xWindow="32130" yWindow="1770" windowWidth="21600" windowHeight="11115" xr2:uid="{29C16FCB-0CAF-4187-9E1B-11F8BF6F8A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -2859,7 +2859,7 @@
         <v>-27.573969999999999</v>
       </c>
       <c r="E71">
-        <v>597325</v>
+        <v>-48.597284999999999</v>
       </c>
       <c r="F71" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
created different files for english and portuguese versions
</commit_message>
<xml_diff>
--- a/features_pontos.xlsx
+++ b/features_pontos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos Mac\ASistemas\Projetos DS\balne_floripa_andhros\Balneabilidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38B8B31-B7CA-4E66-B59F-692DDACB46D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A25555C-6527-4CB1-8803-335708A1CF27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32130" yWindow="1770" windowWidth="21600" windowHeight="11115" xr2:uid="{29C16FCB-0CAF-4187-9E1B-11F8BF6F8A37}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{29C16FCB-0CAF-4187-9E1B-11F8BF6F8A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="138">
   <si>
-    <t>nome</t>
-  </si>
-  <si>
-    <t>referencia</t>
-  </si>
-  <si>
     <t>lat</t>
   </si>
   <si>
@@ -71,21 +65,6 @@
     <t>Em frente à Rua dos Cactos</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>agua_doce</t>
-  </si>
-  <si>
-    <t>desembocadura_praia</t>
-  </si>
-  <si>
-    <t>ponto_perto_desembocadura</t>
-  </si>
-  <si>
-    <t>localizacao</t>
-  </si>
-  <si>
     <t>Não</t>
   </si>
   <si>
@@ -447,6 +426,27 @@
   </si>
   <si>
     <t>Acesso Principal</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>fresh_water</t>
+  </si>
+  <si>
+    <t>drenage_beach</t>
+  </si>
+  <si>
+    <t>drenage_point</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>balneary</t>
   </si>
 </sst>
 </file>
@@ -817,31 +817,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>134</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -849,10 +849,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>-27.611028000000001</v>
@@ -861,16 +861,16 @@
         <v>-48.579740000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -878,10 +878,10 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>-27.616005000000001</v>
@@ -890,16 +890,16 @@
         <v>-48.594940000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -907,10 +907,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>-27.584557</v>
@@ -919,16 +919,16 @@
         <v>-48.549543</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -936,10 +936,10 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>-27.444489000000001</v>
@@ -948,16 +948,16 @@
         <v>-48.524754000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -965,10 +965,10 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>-27.426978999999999</v>
@@ -977,16 +977,16 @@
         <v>-48.464989000000003</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -994,10 +994,10 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>-27.426375</v>
@@ -1006,16 +1006,16 @@
         <v>-48.458444999999998</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1023,10 +1023,10 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>-27.425691</v>
@@ -1035,16 +1035,16 @@
         <v>-48.450294999999997</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1052,10 +1052,10 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>-27.405038000000001</v>
@@ -1064,16 +1064,16 @@
         <v>-48.410227999999996</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1081,10 +1081,10 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>-27.397549999999999</v>
@@ -1093,16 +1093,16 @@
         <v>-48.412864999999996</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1110,10 +1110,10 @@
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>-27.388299</v>
@@ -1122,16 +1122,16 @@
         <v>-48.421225999999997</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1139,10 +1139,10 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D12">
         <v>-27.573336000000001</v>
@@ -1151,16 +1151,16 @@
         <v>-48.423409999999997</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1168,10 +1168,10 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>-27.630013000000002</v>
@@ -1180,16 +1180,16 @@
         <v>-48.448247000000002</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1197,10 +1197,10 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>-27.609113000000001</v>
@@ -1209,16 +1209,16 @@
         <v>-48.444431999999999</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1226,10 +1226,10 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D15">
         <v>-27.604825000000002</v>
@@ -1238,16 +1238,16 @@
         <v>-48.463698000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1255,10 +1255,10 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>-27.608665999999999</v>
@@ -1267,16 +1267,16 @@
         <v>-48.442127999999997</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1284,10 +1284,10 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D17">
         <v>-27.615864999999999</v>
@@ -1296,16 +1296,16 @@
         <v>-48.483783000000003</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1313,10 +1313,10 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D18">
         <v>-27.606535000000001</v>
@@ -1325,16 +1325,16 @@
         <v>-48.461969000000003</v>
       </c>
       <c r="F18" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1342,10 +1342,10 @@
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D19">
         <v>-27.750025999999998</v>
@@ -1354,16 +1354,16 @@
         <v>-48.502654</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1371,10 +1371,10 @@
         <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D20">
         <v>-27.688497999999999</v>
@@ -1383,16 +1383,16 @@
         <v>-48.569040000000001</v>
       </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1400,10 +1400,10 @@
         <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D21">
         <v>-27.67745</v>
@@ -1412,16 +1412,16 @@
         <v>-48.567863000000003</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1429,10 +1429,10 @@
         <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D22">
         <v>-27.426798000000002</v>
@@ -1441,16 +1441,16 @@
         <v>-48.468643</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H22" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1458,10 +1458,10 @@
         <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D23">
         <v>-27.420204999999999</v>
@@ -1470,16 +1470,16 @@
         <v>-48.435346000000003</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H23" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I23" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1487,10 +1487,10 @@
         <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D24">
         <v>-27.426984999999998</v>
@@ -1499,16 +1499,16 @@
         <v>-48.46698</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H24" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1516,10 +1516,10 @@
         <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D25">
         <v>-27.426162999999999</v>
@@ -1528,16 +1528,16 @@
         <v>-48.472926999999999</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G25" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I25" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1545,10 +1545,10 @@
         <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D26">
         <v>-27.608556</v>
@@ -1557,16 +1557,16 @@
         <v>-48.450212000000001</v>
       </c>
       <c r="F26" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H26" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I26" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1574,10 +1574,10 @@
         <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D27">
         <v>-27.605174000000002</v>
@@ -1586,16 +1586,16 @@
         <v>-48.465615999999997</v>
       </c>
       <c r="F27" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G27" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H27" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I27" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1603,10 +1603,10 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D28">
         <v>-27.759910000000001</v>
@@ -1615,16 +1615,16 @@
         <v>-48.572752000000001</v>
       </c>
       <c r="F28" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H28" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1632,10 +1632,10 @@
         <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D29">
         <v>-27.751293</v>
@@ -1644,16 +1644,16 @@
         <v>-48.501291000000002</v>
       </c>
       <c r="F29" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H29" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I29" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1661,10 +1661,10 @@
         <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D30">
         <v>-27.795770999999998</v>
@@ -1673,16 +1673,16 @@
         <v>-48.533738999999997</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G30" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H30" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I30" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1690,10 +1690,10 @@
         <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D31">
         <v>-27.626044</v>
@@ -1702,16 +1702,16 @@
         <v>-48.468325</v>
       </c>
       <c r="F31" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I31" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1719,10 +1719,10 @@
         <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D32">
         <v>-27.40588</v>
@@ -1731,16 +1731,16 @@
         <v>-48.411026999999997</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G32" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H32" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I32" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1748,10 +1748,10 @@
         <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D33">
         <v>-27.625848999999999</v>
@@ -1760,16 +1760,16 @@
         <v>-48.476756999999999</v>
       </c>
       <c r="F33" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H33" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I33" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1777,10 +1777,10 @@
         <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D34">
         <v>-27.726261999999998</v>
@@ -1789,16 +1789,16 @@
         <v>-48.509805</v>
       </c>
       <c r="F34" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H34" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I34" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1806,10 +1806,10 @@
         <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D35">
         <v>-27.393058</v>
@@ -1818,16 +1818,16 @@
         <v>-48.413673000000003</v>
       </c>
       <c r="F35" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G35" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H35" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I35" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -1835,10 +1835,10 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D36">
         <v>-27.423589</v>
@@ -1847,16 +1847,16 @@
         <v>-48.441989999999997</v>
       </c>
       <c r="F36" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G36" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H36" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I36" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -1864,10 +1864,10 @@
         <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D37">
         <v>-27.447517000000001</v>
@@ -1876,16 +1876,16 @@
         <v>-48.535690000000002</v>
       </c>
       <c r="F37" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H37" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I37" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1893,10 +1893,10 @@
         <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D38">
         <v>-27.388625999999999</v>
@@ -1905,16 +1905,16 @@
         <v>-48.426476000000001</v>
       </c>
       <c r="F38" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H38" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I38" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -1922,10 +1922,10 @@
         <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D39">
         <v>-27.571268</v>
@@ -1934,16 +1934,16 @@
         <v>-48.426316</v>
       </c>
       <c r="F39" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G39" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H39" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I39" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1951,10 +1951,10 @@
         <v>92</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D40">
         <v>-27.726148999999999</v>
@@ -1963,16 +1963,16 @@
         <v>-48.505881000000002</v>
       </c>
       <c r="F40" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I40" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1980,10 +1980,10 @@
         <v>94</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D41">
         <v>-27.586434000000001</v>
@@ -1992,16 +1992,16 @@
         <v>-48.553995</v>
       </c>
       <c r="F41" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I41" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -2009,10 +2009,10 @@
         <v>95</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D42">
         <v>-27.583621999999998</v>
@@ -2021,16 +2021,16 @@
         <v>-48.546878</v>
       </c>
       <c r="F42" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H42" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I42" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -2038,10 +2038,10 @@
         <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D43">
         <v>-27.426288</v>
@@ -2050,16 +2050,16 @@
         <v>-48.455103999999999</v>
       </c>
       <c r="F43" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G43" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H43" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I43" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -2067,10 +2067,10 @@
         <v>82</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D44">
         <v>-27.42672</v>
@@ -2079,16 +2079,16 @@
         <v>-48.461607000000001</v>
       </c>
       <c r="F44" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H44" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I44" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -2096,10 +2096,10 @@
         <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D45">
         <v>-27.437698999999999</v>
@@ -2108,16 +2108,16 @@
         <v>-48.490912000000002</v>
       </c>
       <c r="F45" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H45" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I45" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -2125,10 +2125,10 @@
         <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D46">
         <v>-27.437961999999999</v>
@@ -2137,16 +2137,16 @@
         <v>-48.486347000000002</v>
       </c>
       <c r="F46" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G46" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H46" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I46" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -2154,10 +2154,10 @@
         <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D47">
         <v>-27.437287000000001</v>
@@ -2166,16 +2166,16 @@
         <v>-48.482855000000001</v>
       </c>
       <c r="F47" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G47" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H47" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I47" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -2183,10 +2183,10 @@
         <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D48">
         <v>-27.431652</v>
@@ -2195,16 +2195,16 @@
         <v>-48.479799999999997</v>
       </c>
       <c r="F48" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G48" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H48" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I48" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -2212,10 +2212,10 @@
         <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D49">
         <v>-27.432300999999999</v>
@@ -2224,16 +2224,16 @@
         <v>-48.513193000000001</v>
       </c>
       <c r="F49" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G49" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H49" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I49" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -2241,10 +2241,10 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D50">
         <v>-27.436655999999999</v>
@@ -2253,16 +2253,16 @@
         <v>-48.501671999999999</v>
       </c>
       <c r="F50" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G50" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H50" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I50" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2270,10 +2270,10 @@
         <v>23</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C51" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D51">
         <v>-27.395641000000001</v>
@@ -2282,16 +2282,16 @@
         <v>-48.434984999999998</v>
       </c>
       <c r="F51" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G51" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H51" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I51" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -2299,10 +2299,10 @@
         <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C52" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D52">
         <v>-27.434404000000001</v>
@@ -2311,16 +2311,16 @@
         <v>-48.508766999999999</v>
       </c>
       <c r="F52" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G52" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H52" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I52" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -2328,10 +2328,10 @@
         <v>67</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D53">
         <v>-27.403108</v>
@@ -2340,16 +2340,16 @@
         <v>-48.427827000000001</v>
       </c>
       <c r="F53" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G53" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H53" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I53" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -2357,10 +2357,10 @@
         <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D54">
         <v>-27.413594</v>
@@ -2369,16 +2369,16 @@
         <v>-48.428657999999999</v>
       </c>
       <c r="F54" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G54" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H54" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I54" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -2386,10 +2386,10 @@
         <v>83</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C55" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D55">
         <v>-27.413719</v>
@@ -2398,16 +2398,16 @@
         <v>-48.428100000000001</v>
       </c>
       <c r="F55" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H55" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I55" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2415,10 +2415,10 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C56" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D56">
         <v>-27.494629</v>
@@ -2427,16 +2427,16 @@
         <v>-48.525491000000002</v>
       </c>
       <c r="F56" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G56" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H56" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I56" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -2444,10 +2444,10 @@
         <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C57" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D57">
         <v>-27.489332000000001</v>
@@ -2456,16 +2456,16 @@
         <v>-48.538093000000003</v>
       </c>
       <c r="F57" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G57" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H57" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I57" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -2473,10 +2473,10 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D58">
         <v>-27.507729000000001</v>
@@ -2485,16 +2485,16 @@
         <v>-48.520074000000001</v>
       </c>
       <c r="F58" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G58" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H58" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I58" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -2502,10 +2502,10 @@
         <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C59" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D59">
         <v>-27.505351000000001</v>
@@ -2514,16 +2514,16 @@
         <v>-48.522652000000001</v>
       </c>
       <c r="F59" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G59" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H59" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I59" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -2531,10 +2531,10 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C60" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D60">
         <v>-27.577916999999999</v>
@@ -2543,16 +2543,16 @@
         <v>-48.578470000000003</v>
       </c>
       <c r="F60" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G60" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H60" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I60" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -2560,10 +2560,10 @@
         <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C61" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D61">
         <v>-27.612113000000001</v>
@@ -2572,16 +2572,16 @@
         <v>-48.596888</v>
       </c>
       <c r="F61" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G61" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H61" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I61" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -2589,10 +2589,10 @@
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D62">
         <v>-27.532475000000002</v>
@@ -2601,16 +2601,16 @@
         <v>-48.525410999999998</v>
       </c>
       <c r="F62" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G62" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H62" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I62" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -2618,10 +2618,10 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C63" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D63">
         <v>-27.542473999999999</v>
@@ -2630,16 +2630,16 @@
         <v>-48.524731000000003</v>
       </c>
       <c r="F63" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G63" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H63" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I63" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -2647,10 +2647,10 @@
         <v>35</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C64" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D64">
         <v>-27.690052999999999</v>
@@ -2659,16 +2659,16 @@
         <v>-48.481163000000002</v>
       </c>
       <c r="F64" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G64" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H64" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I64" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -2676,10 +2676,10 @@
         <v>73</v>
       </c>
       <c r="B65" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C65" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D65">
         <v>-27.685894000000001</v>
@@ -2688,16 +2688,16 @@
         <v>-48.480992999999998</v>
       </c>
       <c r="F65" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G65" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H65" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I65" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -2705,10 +2705,10 @@
         <v>75</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C66" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D66">
         <v>-27.687170999999999</v>
@@ -2717,16 +2717,16 @@
         <v>-48.480612000000001</v>
       </c>
       <c r="F66" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G66" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H66" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I66" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -2734,10 +2734,10 @@
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C67" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D67">
         <v>-27.433803000000001</v>
@@ -2746,16 +2746,16 @@
         <v>-48.519793</v>
       </c>
       <c r="F67" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G67" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H67" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I67" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -2763,10 +2763,10 @@
         <v>89</v>
       </c>
       <c r="B68" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C68" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D68">
         <v>-27.669295000000002</v>
@@ -2775,16 +2775,16 @@
         <v>-48.476435000000002</v>
       </c>
       <c r="F68" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G68" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H68" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I68" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
@@ -2792,10 +2792,10 @@
         <v>90</v>
       </c>
       <c r="B69" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" t="s">
         <v>101</v>
-      </c>
-      <c r="C69" t="s">
-        <v>108</v>
       </c>
       <c r="D69">
         <v>-27.697800999999998</v>
@@ -2804,16 +2804,16 @@
         <v>-48.489634000000002</v>
       </c>
       <c r="F69" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G69" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H69" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I69" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
@@ -2821,10 +2821,10 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C70" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D70">
         <v>-27.616880999999999</v>
@@ -2833,16 +2833,16 @@
         <v>-48.591920000000002</v>
       </c>
       <c r="F70" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G70" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H70" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I70" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -2850,10 +2850,10 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C71" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D71">
         <v>-27.573969999999999</v>
@@ -2862,16 +2862,16 @@
         <v>-48.597284999999999</v>
       </c>
       <c r="F71" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G71" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H71" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I71" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -2879,10 +2879,10 @@
         <v>52</v>
       </c>
       <c r="B72" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C72" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D72">
         <v>-27.61289</v>
@@ -2891,16 +2891,16 @@
         <v>-48.547490000000003</v>
       </c>
       <c r="F72" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G72" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H72" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I72" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
@@ -2908,10 +2908,10 @@
         <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C73" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D73">
         <v>-27.586949000000001</v>
@@ -2920,16 +2920,16 @@
         <v>-48.576583999999997</v>
       </c>
       <c r="F73" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G73" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H73" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I73" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -2937,10 +2937,10 @@
         <v>5</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C74" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D74">
         <v>-27.613503000000001</v>
@@ -2949,16 +2949,16 @@
         <v>-48.58502</v>
       </c>
       <c r="F74" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G74" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H74" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I74" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -2966,10 +2966,10 @@
         <v>45</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C75" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D75">
         <v>-27.782581</v>
@@ -2978,16 +2978,16 @@
         <v>-48.508263999999997</v>
       </c>
       <c r="F75" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G75" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H75" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I75" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -2995,10 +2995,10 @@
         <v>87</v>
       </c>
       <c r="B76" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C76" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D76">
         <v>-27.504877</v>
@@ -3007,16 +3007,16 @@
         <v>-48.404209000000002</v>
       </c>
       <c r="F76" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G76" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H76" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I76" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -3024,10 +3024,10 @@
         <v>91</v>
       </c>
       <c r="B77" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C77" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D77">
         <v>-27.717661</v>
@@ -3036,16 +3036,16 @@
         <v>-48.503337999999999</v>
       </c>
       <c r="F77" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G77" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H77" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I77" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -3053,10 +3053,10 @@
         <v>47</v>
       </c>
       <c r="B78" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C78" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D78">
         <v>-27.719104000000002</v>
@@ -3065,16 +3065,16 @@
         <v>-48.564481000000001</v>
       </c>
       <c r="F78" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G78" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H78" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I78" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -3082,10 +3082,10 @@
         <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C79" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D79">
         <v>-27.784081</v>
@@ -3094,16 +3094,16 @@
         <v>-48.523780000000002</v>
       </c>
       <c r="F79" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G79" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H79" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I79" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -3111,10 +3111,10 @@
         <v>31</v>
       </c>
       <c r="B80" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C80" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D80">
         <v>-27.463459</v>
@@ -3123,16 +3123,16 @@
         <v>-48.376213</v>
       </c>
       <c r="F80" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G80" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H80" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I80" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -3140,10 +3140,10 @@
         <v>27</v>
       </c>
       <c r="B81" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C81" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D81">
         <v>-27.425568999999999</v>
@@ -3152,16 +3152,16 @@
         <v>-48.398539999999997</v>
       </c>
       <c r="F81" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G81" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H81" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I81" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -3169,10 +3169,10 @@
         <v>28</v>
       </c>
       <c r="B82" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C82" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D82">
         <v>-27.435925999999998</v>
@@ -3181,16 +3181,16 @@
         <v>-48.390647999999999</v>
       </c>
       <c r="F82" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G82" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H82" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I82" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
@@ -3198,10 +3198,10 @@
         <v>29</v>
       </c>
       <c r="B83" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C83" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D83">
         <v>-27.443462</v>
@@ -3210,16 +3210,16 @@
         <v>-48.376631000000003</v>
       </c>
       <c r="F83" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G83" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H83" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I83" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
@@ -3227,10 +3227,10 @@
         <v>57</v>
       </c>
       <c r="B84" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C84" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D84">
         <v>-27.439036999999999</v>
@@ -3239,16 +3239,16 @@
         <v>-48.386766000000001</v>
       </c>
       <c r="F84" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G84" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H84" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I84" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -3256,10 +3256,10 @@
         <v>58</v>
       </c>
       <c r="B85" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C85" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D85">
         <v>-27.433592999999998</v>
@@ -3268,16 +3268,16 @@
         <v>-48.392997999999999</v>
       </c>
       <c r="F85" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G85" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H85" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I85" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -3285,10 +3285,10 @@
         <v>77</v>
       </c>
       <c r="B86" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C86" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D86">
         <v>-27.420408999999999</v>
@@ -3297,16 +3297,16 @@
         <v>-48.401698000000003</v>
       </c>
       <c r="F86" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G86" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H86" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I86" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -3314,10 +3314,10 @@
         <v>78</v>
       </c>
       <c r="B87" t="s">
+        <v>121</v>
+      </c>
+      <c r="C87" t="s">
         <v>128</v>
-      </c>
-      <c r="C87" t="s">
-        <v>135</v>
       </c>
       <c r="D87">
         <v>-27.435669000000001</v>
@@ -3326,16 +3326,16 @@
         <v>-48.390909999999998</v>
       </c>
       <c r="F87" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G87" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H87" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I87" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
@@ -3343,10 +3343,10 @@
         <v>71</v>
       </c>
       <c r="B88" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C88" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D88">
         <v>-27.603588999999999</v>
@@ -3355,16 +3355,16 @@
         <v>-48.433155999999997</v>
       </c>
       <c r="F88" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G88" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H88" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I88" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>